<commit_message>
Updated status bar and file names Modified the errors
</commit_message>
<xml_diff>
--- a/excelfiles/count_of_linktypes.xlsx
+++ b/excelfiles/count_of_linktypes.xlsx
@@ -7,8 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Link Counts" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Link Details" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,7 +441,22 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Count</t>
+          <t>By part</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Partseries</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Blanket</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>count</t>
         </is>
       </c>
     </row>
@@ -455,6 +469,15 @@
       <c r="B2" t="n">
         <v>3</v>
       </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -465,6 +488,15 @@
       <c r="B3" t="n">
         <v>2</v>
       </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -475,6 +507,15 @@
       <c r="B4" t="n">
         <v>2</v>
       </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -483,6 +524,15 @@
         </is>
       </c>
       <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" t="n">
         <v>5</v>
       </c>
     </row>
@@ -495,6 +545,15 @@
       <c r="B6" t="n">
         <v>1</v>
       </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -505,6 +564,15 @@
       <c r="B7" t="n">
         <v>1</v>
       </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -515,6 +583,15 @@
       <c r="B8" t="n">
         <v>5</v>
       </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -525,6 +602,15 @@
       <c r="B9" t="n">
         <v>2</v>
       </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -535,6 +621,15 @@
       <c r="B10" t="n">
         <v>1</v>
       </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -545,6 +640,15 @@
       <c r="B11" t="n">
         <v>1</v>
       </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -555,6 +659,15 @@
       <c r="B12" t="n">
         <v>2</v>
       </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -563,6 +676,15 @@
         </is>
       </c>
       <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" t="n">
         <v>2</v>
       </c>
     </row>
@@ -575,6 +697,15 @@
       <c r="B14" t="n">
         <v>1</v>
       </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -585,6 +716,15 @@
       <c r="B15" t="n">
         <v>1</v>
       </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -595,6 +735,15 @@
       <c r="B16" t="n">
         <v>1</v>
       </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -603,6 +752,15 @@
         </is>
       </c>
       <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
         <v>2</v>
       </c>
     </row>
@@ -615,6 +773,15 @@
       <c r="B18" t="n">
         <v>1</v>
       </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -625,6 +792,15 @@
       <c r="B19" t="n">
         <v>1</v>
       </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -635,6 +811,15 @@
       <c r="B20" t="n">
         <v>1</v>
       </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -645,6 +830,15 @@
       <c r="B21" t="n">
         <v>1</v>
       </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -655,6 +849,15 @@
       <c r="B22" t="n">
         <v>1</v>
       </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -665,6 +868,15 @@
       <c r="B23" t="n">
         <v>1</v>
       </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -675,6 +887,15 @@
       <c r="B24" t="n">
         <v>1</v>
       </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -685,6 +906,15 @@
       <c r="B25" t="n">
         <v>1</v>
       </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -693,285 +923,15 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B26"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>index</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>http://192.168.20.216/sample-docs/03-11-2024/Bourns/Bourns_SF-Series_ROHS.pdf</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>https://ilensysin-my.sharepoint.com/personal/mohanvamsi_sadhu_ilensys_in/_layouts/15/onedrive.aspx?id=%2Fpersonal%2Fmohanvamsi%5Fsadhu%5Filensys%5Fin%2FDocuments%2FFeuerherdt%5FREACH%2Epdf&amp;parent=%2Fpersonal%2Fmohanvamsi%5Fsadhu%5Filensys%5Fin%2FDocuments</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>http://192.168.20.216/sample-docs/02-18-2024/Ettinger/063.32.170_ROHS,REACH.pdf</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>http://192.168.20.216/sample-docs/02-18-2024/Feuerherdt/Feuerherdt_REACH.pdf</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>http://192.168.20.216/sample-docs/02-18-2024/Ettinger/013.14.235_ROHS,REACH.pdf</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>http://192.168.20.216/sample-docs/02-18-2024/Ettinger/02.17.149_ROHS,REACH.pdf</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>https://ilensysin-my.sharepoint.com/personal/mohanvamsi_sadhu_ilensys_in/_layouts/15/onedrive.aspx?id=%2Fpersonal%2Fmohanvamsi%5Fsadhu%5Filensys%5Fin%2FDocuments%2FEU%5FREACH%2D219%2Ditem%2D2021%2D07%2D08%2Epdf&amp;parent=%2Fpersonal%2Fmohanvamsi%5Fsadhu%5Fil</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>http://192.168.20.216/sample-docs/02-18-2024/Ettinger/03.20.059_ROHS,REACH.pdf</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>http://192.168.20.216/sample-docs/02-18-2024/Ettinger/013.13.825_ROHS,REACH.pdf</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>https://ilensysin-my.sharepoint.com/personal/mohanvamsi_sadhu_ilensys_in/_layouts/15/onedrive.aspx?id=%2Fpersonal%2Fmohanvamsi%5Fsadhu%5Filensys%5Fin%2FDocuments%2F76347%2D301LF%2Epdf&amp;parent=%2Fpersonal%2Fmohanvamsi%5Fsadhu%5Filensys%5Fin%2FDocuments</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>http://192.168.20.216/sample-docs/03-11-2024/Amphenol/76347-301LF.pdf</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>http://192.168.20.216/sample-docs/02-18-2024/Ettinger/03.03.045_ROHS,REACH.pdf</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>http://192.168.20.216/sample-docs/02-18-2024/Ettinger/05.07.053_ROHS,REACH.pdf</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>https://ilensysin-my.sharepoint.com/:b:/g/personal/mohanvamsi_sadhu_ilensys_in/EY_ASdWhPQlJmqcXtF-zGwcB-4EtN8xPDiK1yYmpJ8BxEw?e=9HHjDX</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>http://192.168.20.216/sample-docs/02-18-2024/Ettinger/01.63.232_ROHS,REACH.pdf</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>http://192.168.20.216/sample-docs/03-11-2024/Bourns/3386_250-50k_mds.pdf</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>http://192.168.20.216/sample-docs/03-11-2024/Amp/34148-0_ROHS,REACH.pdf</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>http://192.168.20.216/sample-docs/02-18-2024/Ettinger/03.73.151_ROHS,REACH.pdf</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>http://192.168.20.216/sample-docs/02-18-2024/Ettinger/05.03.251_ROHS,REACH.pdf</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>http://192.168.20.216/sample-docs/02-18-2024/Ettinger/01.26.142_ROHS,REACH.pdf</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>http://192.168.20.216/sample-docs/03-11-2024/Bourns/4607x_mds.pdf</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>http://192.168.20.216/sample-docs/02-18-2024/Epcos/B82111E%20SERIES.pdf</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>http://192.168.20.216/sample-docs/02-18-2024/Ettinger/034.18.024_ROHS,REACH.pdf</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>http://192.168.20.216/sample-docs/03-11-2024/Bourns/SMCJ1_MDS.pdf</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>http://192.168.20.216/sample-docs/02-18-2024/E-Tec/EU_REACH-219-item-2021-07-08.pdf</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>